<commit_message>
1ere version avec gradio
</commit_message>
<xml_diff>
--- a/classements_xls633be4e053e80.xlsx
+++ b/classements_xls633be4e053e80.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>P11/P10/P11</t>
+          <t>P11/P10/P10</t>
         </is>
       </c>
     </row>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>D9/D9/D9</t>
+          <t>D9/D8/D9</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>D7/D7/D7</t>
+          <t>D7/D7/R6</t>
         </is>
       </c>
     </row>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>P10/P11/P11</t>
+          <t>P10/P10/P11</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>P11/P10/D9</t>
+          <t>P10/P10/D9</t>
         </is>
       </c>
     </row>

</xml_diff>